<commit_message>
Aggiornati gli xlsx controllata dimensione intervallo di confidenza aggiunto grafico sul tempo globale nel capitolo 10, paragrafo orizzonte finito
</commit_message>
<xml_diff>
--- a/analysis/steady_state/xlsx/base_steady_state_017.xlsx
+++ b/analysis/steady_state/xlsx/base_steady_state_017.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wronek\Documents\1) Università\Magistrale\Anno 2022-2023\Semestre 2\PMCSN\Project\analysis\steady_state\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wronek\Documents\1 - Università\Magistrale\Anno 2022-2023\Semestre 2\PMCSN\Project\analysis\steady_state\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3281FCE-905E-4CC4-AC12-0EF25DEF8497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC67A37-7125-46C9-AABE-1C0642E30E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2415" windowWidth="28665" windowHeight="18465"/>
+    <workbookView xWindow="0" yWindow="3120" windowWidth="38400" windowHeight="18465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_steady_state_017" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="17">
   <si>
-    <t>Based on a simulation splitted into 200 batches and with 99.00% confidence</t>
-  </si>
-  <si>
     <t>NODE 1</t>
   </si>
   <si>
@@ -71,12 +68,15 @@
   </si>
   <si>
     <t>Average max response time:</t>
+  </si>
+  <si>
+    <t>Based on a simulation splitted into 64 batches and with 95.00% confidence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -562,9 +562,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -572,6 +569,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -928,538 +928,538 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.52637500000000004</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="1">
+        <v>0.527084</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.16E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3">
-        <v>1.6000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="1">
+        <v>10.713075999999999</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.72724900000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3">
-        <v>10.785228999999999</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B6" s="1">
+        <v>8.7133450000000003</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.72462300000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.9997100000000001</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4.6490000000000004E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>20.371434000000001</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.3896379999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>16.569862000000001</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.383696</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.95038299999999998</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2.33E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.84970500000000004</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2.3059999999999999E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="3">
-        <v>0.1231</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="B15" s="1">
+        <v>15.072952000000001</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1.0235000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1">
+        <v>11.867770999999999</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.018367</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3">
-        <v>8.7856670000000001</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B17" s="1">
+        <v>3.2051509999999999</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>8.3320000000000009E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1">
+        <v>17.791919</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.2251399999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1">
+        <v>14.012060999999999</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.2157169999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.94495600000000002</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3.0720000000000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.3234859999999999</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="1">
+        <v>4.5259999999999996E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3">
-        <v>0.12278500000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="B25" s="1">
+        <v>22.080546999999999</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2.2682199999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="1">
+        <v>19.581066</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2.263099</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2.4994670000000001</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="1">
+        <v>8.7709999999999993E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3">
-        <v>1.9995620000000001</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B28" s="1">
+        <v>16.751418999999999</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1.7468410000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1">
+        <v>14.858862</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1.74061</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.94627300000000003</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="1">
+        <v>4.2599999999999999E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.65066199999999996</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1.8060000000000001E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3">
-        <v>5.8699999999999996E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="B35" s="1">
+        <v>5.660266</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2.1918E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="1">
+        <v>4.3617119999999998</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1.8363000000000001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1.2985519999999999</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="1">
+        <v>3.6879999999999999E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="1">
+        <v>8.7160189999999993</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1.3919000000000001E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3">
-        <v>20.491759999999999</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.23457700000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B39" s="1">
+        <v>6.7163069999999996</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1.1594E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3">
-        <v>16.692665000000002</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.233852</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="B40" s="1">
+        <v>0.99985500000000005</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1.836E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3">
-        <v>0.94977400000000001</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="3">
-        <v>3.3199999999999999E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3">
-        <v>0.847526</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="3">
-        <v>3.6900000000000002E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="3">
-        <v>15.709376000000001</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.21115500000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3">
-        <v>12.509269</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.21049499999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="3">
-        <v>3.2001059999999999</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="3">
-        <v>1.2669999999999999E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="3">
-        <v>18.538526999999998</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.25232300000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="3">
-        <v>14.762340999999999</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0.25092799999999998</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="3">
-        <v>0.94404600000000005</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="3">
-        <v>4.9799999999999996E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="4">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="3">
-        <v>1.321021</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="3">
-        <v>6.5600000000000001E-4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="3">
-        <v>23.710621</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0.40712599999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="3">
-        <v>21.210868000000001</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0.406364</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="3">
-        <v>2.4997530000000001</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="3">
-        <v>1.2830000000000001E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="3">
-        <v>17.951687</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="3">
-        <v>0.31097200000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="3">
-        <v>16.059211000000001</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="3">
-        <v>0.31013200000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="3">
-        <v>0.94623800000000002</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="3">
-        <v>6.1499999999999999E-4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="4">
-        <v>0</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="B41" s="3">
+        <v>0.42955300000000002</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1.934E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="3">
-        <v>0.65140699999999996</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="3">
-        <v>2.23E-4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="3">
-        <v>5.6698979999999999</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="3">
-        <v>2.6689999999999999E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="3">
-        <v>4.3698990000000002</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="3">
-        <v>2.2390000000000001E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="3">
-        <v>1.2999989999999999</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="3">
-        <v>4.5100000000000001E-4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" s="3">
-        <v>8.704879</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="3">
-        <v>2.1580000000000002E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="3">
-        <v>6.7090129999999997</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="3">
-        <v>1.755E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="3">
-        <v>0.99793299999999996</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="3">
-        <v>2.72E-4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" s="4">
-        <v>0.43137500000000001</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="4">
-        <v>2.4800000000000001E-4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="3">
-        <v>55.875100000000003</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="3">
-        <v>0.53349999999999997</v>
+      <c r="B43" s="1">
+        <v>53.526800000000001</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2.6678000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>